<commit_message>
S & O Finished
</commit_message>
<xml_diff>
--- a/Documentation/AI Information/Behaviour Flow & State Diagrams.xlsx
+++ b/Documentation/AI Information/Behaviour Flow & State Diagrams.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28421"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="25600" windowHeight="16000" tabRatio="500" firstSheet="2" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14580" tabRatio="500" firstSheet="4" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Light Demon" sheetId="1" r:id="rId1"/>
@@ -15,6 +15,8 @@
     <sheet name="Ghost" sheetId="5" r:id="rId6"/>
     <sheet name="Main Character" sheetId="7" r:id="rId7"/>
     <sheet name="Main Character Sub" sheetId="8" r:id="rId8"/>
+    <sheet name="Saving" sheetId="9" r:id="rId9"/>
+    <sheet name="Main UML" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -77,8 +79,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="135">
+  <cellStyleXfs count="157">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -217,7 +241,7 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="135">
+  <cellStyles count="157">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -285,6 +309,17 @@
     <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -352,6 +387,17 @@
     <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -5253,6 +5299,1743 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>698500</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>558800</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Oval 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3175000" y="2286000"/>
+          <a:ext cx="1511300" cy="1308100"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" b="1"/>
+            <a:t>Project</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" b="1" baseline="0"/>
+            <a:t> Night Terror</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1600" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>749300</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>368300</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Oval 5"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3225800" y="393700"/>
+          <a:ext cx="1270000" cy="1193800"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" b="1"/>
+            <a:t>Game State</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>711200</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="Oval 10"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6946900" y="457200"/>
+          <a:ext cx="1193800" cy="1092200"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="1"/>
+            <a:t>Blueprints</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1000" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="Oval 13"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5384800" y="1651000"/>
+          <a:ext cx="1270000" cy="1193800"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" b="1"/>
+            <a:t>Level</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="Oval 14"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1651000" y="381000"/>
+          <a:ext cx="1270000" cy="1193800"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" b="1"/>
+            <a:t>Game Mode</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>368300</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>736600</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="32" name="Oval 31"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6972300" y="1714500"/>
+          <a:ext cx="1193800" cy="1092200"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="1"/>
+            <a:t>Static Meshes</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1000" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>787400</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="41" name="Oval 40"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7023100" y="2997200"/>
+          <a:ext cx="1193800" cy="1092200"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="1"/>
+            <a:t>Other</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1000" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>660400</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="48" name="Oval 47"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3136900" y="4813300"/>
+          <a:ext cx="1422400" cy="1308100"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" b="1"/>
+            <a:t>Character</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>261620</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="69" name="Frame 68"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5214620" y="355600"/>
+          <a:ext cx="3129280" cy="3848100"/>
+        </a:xfrm>
+        <a:prstGeom prst="frame">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 0"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="square"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>749300</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="70" name="Frame 69"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1574800" y="317500"/>
+          <a:ext cx="2997200" cy="1371600"/>
+        </a:xfrm>
+        <a:prstGeom prst="frame">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 0"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="square"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>698500</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="74" name="TextBox 73"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2349500" y="76200"/>
+          <a:ext cx="1536700" cy="317500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>Game Settings &amp; Info</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="75" name="TextBox 74"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6108700" y="139700"/>
+          <a:ext cx="1536700" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>Level Settings</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="77" name="Oval 76"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="762000" y="5295900"/>
+          <a:ext cx="1206500" cy="1130300"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="1"/>
+            <a:t>Animation Blueprint</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1000" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="80" name="Oval 79"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="762000" y="6756400"/>
+          <a:ext cx="1206500" cy="1130300"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="1"/>
+            <a:t>Blend Space</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1000" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="86" name="Frame 85"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="723900" y="5232400"/>
+          <a:ext cx="1346200" cy="2755900"/>
+        </a:xfrm>
+        <a:prstGeom prst="frame">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 0"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="square"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>292100</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="100" name="TextBox 99"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="863600" y="5029200"/>
+          <a:ext cx="1079500" cy="254000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>Animation</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="109" name="Oval 108"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4622800" y="6705600"/>
+          <a:ext cx="1206500" cy="1130300"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="1"/>
+            <a:t>Meshes</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1000" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>749300</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="110" name="Oval 109"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3225800" y="6667500"/>
+          <a:ext cx="1206500" cy="1130300"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="1"/>
+            <a:t>Blueprints</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1000" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>539750</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>539750</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="112" name="Straight Arrow Connector 111"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="80" idx="0"/>
+          <a:endCxn id="77" idx="4"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1365250" y="6426200"/>
+          <a:ext cx="0" cy="330200"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>690313</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>2972</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>593928</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>109149</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="115" name="Straight Arrow Connector 114"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="41" idx="1"/>
+          <a:endCxn id="14" idx="5"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="6468813" y="2669972"/>
+          <a:ext cx="729115" cy="487177"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>368300</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="118" name="Straight Arrow Connector 117"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="32" idx="2"/>
+          <a:endCxn id="14" idx="6"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="6654800" y="2247900"/>
+          <a:ext cx="317500" cy="12700"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>690313</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>55951</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>517728</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>111328</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="121" name="Straight Arrow Connector 120"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="11" idx="3"/>
+          <a:endCxn id="14" idx="7"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6468813" y="1389451"/>
+          <a:ext cx="652915" cy="436377"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>24333</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>43206</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="124" name="Straight Arrow Connector 123"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="86" idx="3"/>
+          <a:endCxn id="48" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2070100" y="5929833"/>
+          <a:ext cx="1275106" cy="680517"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>628650</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>635000</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="127" name="Straight Arrow Connector 126"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="166" idx="0"/>
+          <a:endCxn id="2" idx="4"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="3930650" y="3594100"/>
+          <a:ext cx="6350" cy="1130300"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>337475</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>261620</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>1067</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="130" name="Straight Arrow Connector 129"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="69" idx="1"/>
+          <a:endCxn id="2" idx="7"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="4464975" y="2279650"/>
+          <a:ext cx="749645" cy="197917"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>596900</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>94325</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>1067</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="133" name="Straight Arrow Connector 132"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="70" idx="2"/>
+          <a:endCxn id="2" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3073400" y="1689100"/>
+          <a:ext cx="322925" cy="788467"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>223494</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>24333</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="137" name="Straight Arrow Connector 136"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="155" idx="0"/>
+          <a:endCxn id="48" idx="5"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="4350994" y="5929833"/>
+          <a:ext cx="856006" cy="674167"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="149" name="Oval 148"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6007100" y="6692900"/>
+          <a:ext cx="1206500" cy="1130300"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="1"/>
+            <a:t>Other</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1000" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>673100</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>660400</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="155" name="Frame 154"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3149600" y="6604000"/>
+          <a:ext cx="4114800" cy="1295400"/>
+        </a:xfrm>
+        <a:prstGeom prst="frame">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 0"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="square"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>520700</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>774700</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="158" name="TextBox 157"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4648200" y="6426200"/>
+          <a:ext cx="1079500" cy="254000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>Components</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>508000</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="166" name="Frame 165"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="508000" y="4724400"/>
+          <a:ext cx="6858000" cy="3327400"/>
+        </a:xfrm>
+        <a:prstGeom prst="frame">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 0"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="square"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>774700</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="167" name="TextBox 166"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4902200" y="4635500"/>
+          <a:ext cx="1079500" cy="254000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>Characters</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -20197,6 +21980,1390 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="64" name="TextBox 63"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19177000" y="2159000"/>
+          <a:ext cx="1219200" cy="520700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Load </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>Started</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="65" name="TextBox 64"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4775200" y="736600"/>
+          <a:ext cx="1536700" cy="317500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Check if Save Exists</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="96" name="TextBox 95"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8077200" y="736600"/>
+          <a:ext cx="1536700" cy="317500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Do Nothing</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="102" name="Straight Connector 101"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="64" idx="3"/>
+          <a:endCxn id="65" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3886200" y="895350"/>
+          <a:ext cx="889000" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle" w="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="105" name="Straight Connector 104"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="65" idx="3"/>
+          <a:endCxn id="96" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6311900" y="895350"/>
+          <a:ext cx="1765300" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle" w="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="111" name="TextBox 110"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6794500" y="736600"/>
+          <a:ext cx="711200" cy="317500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>No Save</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>577850</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="112" name="Straight Connector 111"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="65" idx="2"/>
+          <a:endCxn id="115" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="5530850" y="1054100"/>
+          <a:ext cx="12700" cy="952500"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle" w="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>635000</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>520700</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="115" name="TextBox 114"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4762500" y="2006600"/>
+          <a:ext cx="1536700" cy="698500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Copy Save</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> File Variables into Current Game Varaibles</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="119" name="TextBox 118"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2667000" y="635000"/>
+          <a:ext cx="1219200" cy="520700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Save </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>Started</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="120" name="TextBox 119"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4775200" y="736600"/>
+          <a:ext cx="1536700" cy="317500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Check if Save Exists</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="123" name="TextBox 122"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8077200" y="736600"/>
+          <a:ext cx="1536700" cy="317500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Create New</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> Save File</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="124" name="Straight Connector 123"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="119" idx="3"/>
+          <a:endCxn id="120" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3886200" y="895350"/>
+          <a:ext cx="889000" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle" w="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="125" name="Straight Connector 124"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="120" idx="3"/>
+          <a:endCxn id="123" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6311900" y="895350"/>
+          <a:ext cx="1765300" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle" w="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="126" name="TextBox 125"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6794500" y="736600"/>
+          <a:ext cx="711200" cy="317500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>No Save</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>577850</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>577850</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="127" name="Straight Connector 126"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="135" idx="2"/>
+          <a:endCxn id="128" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5530850" y="4940300"/>
+          <a:ext cx="0" cy="749300"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle" w="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>635000</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>520700</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="128" name="TextBox 127"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4762500" y="5689600"/>
+          <a:ext cx="1536700" cy="698500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Copy Current </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>Game Variables into Save File Varaibles</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="129" name="TextBox 128"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5016500" y="1435100"/>
+          <a:ext cx="1028700" cy="228600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Save exists</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>635000</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>520700</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="135" name="TextBox 134"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4762500" y="4483100"/>
+          <a:ext cx="1536700" cy="457200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Prompt</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> User to Overwrite Current Save</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>577850</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="136" name="Straight Connector 135"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="120" idx="2"/>
+          <a:endCxn id="135" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="5530850" y="3721100"/>
+          <a:ext cx="12700" cy="762000"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle" w="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="147" name="TextBox 146"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5003800" y="3987800"/>
+          <a:ext cx="1028700" cy="228600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Save exists</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="149" name="TextBox 148"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5003800" y="5156200"/>
+          <a:ext cx="1079500" cy="279400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>Player Says Yes</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>520700</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>711200</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="150" name="Straight Connector 149"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="135" idx="3"/>
+          <a:endCxn id="154" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6299200" y="4711700"/>
+          <a:ext cx="1841500" cy="19050"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle" w="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>711200</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>596900</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="154" name="TextBox 153"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8140700" y="4572000"/>
+          <a:ext cx="1536700" cy="317500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Do Nothing</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="157" name="TextBox 156"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6616700" y="4584700"/>
+          <a:ext cx="1079500" cy="279400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>Player Says No</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>520700</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="159" name="Straight Connector 158"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="123" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6299200" y="3721100"/>
+          <a:ext cx="2546350" cy="762000"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle" w="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -20526,8 +23693,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="R5" workbookViewId="0">
-      <selection activeCell="V6" sqref="V6:AD42"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A8" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:K43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -20589,7 +23777,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -20610,8 +23798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:XFD33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -20679,7 +23867,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F2" workbookViewId="0">
+    <sheetView topLeftCell="F2" workbookViewId="0">
       <selection activeCell="O32" sqref="O32"/>
     </sheetView>
   </sheetViews>
@@ -20694,4 +23882,25 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>